<commit_message>
Finition de l'algorithme qui déplace un à la fois
</commit_message>
<xml_diff>
--- a/Planning_CVRP.xlsx
+++ b/Planning_CVRP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Programming\C#\TPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Programming\C#\TPI\git\CVRP_Viewer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81751C4B-BAB2-484B-B5A0-B6FB8807F232}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EF4995-8A66-417F-8ACE-E971378739F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C268FC12-0260-4BE3-B295-C69B9861881F}"/>
   </bookViews>
@@ -332,26 +332,26 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -680,10 +680,10 @@
   <dimension ref="A1:Y62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S35" sqref="S35"/>
+      <selection pane="bottomRight" activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,138 +717,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="20"/>
+      <c r="F2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="14" t="s">
+      <c r="G2" s="20"/>
+      <c r="H2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="14" t="s">
+      <c r="I2" s="20"/>
+      <c r="J2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="14" t="s">
+      <c r="K2" s="20"/>
+      <c r="L2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="14" t="s">
+      <c r="M2" s="20"/>
+      <c r="N2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="15"/>
-      <c r="P2" s="14" t="s">
+      <c r="O2" s="20"/>
+      <c r="P2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="14" t="s">
+      <c r="Q2" s="20"/>
+      <c r="R2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="15"/>
-      <c r="T2" s="14" t="s">
+      <c r="S2" s="20"/>
+      <c r="T2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="14" t="s">
+      <c r="U2" s="20"/>
+      <c r="V2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="15"/>
-      <c r="X2" s="14" t="s">
+      <c r="W2" s="20"/>
+      <c r="X2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="Y2" s="15"/>
+      <c r="Y2" s="20"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="18">
+      <c r="A3" s="17"/>
+      <c r="B3" s="15">
         <v>43976</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="18">
+      <c r="C3" s="16"/>
+      <c r="D3" s="15">
         <v>43977</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="18">
+      <c r="E3" s="16"/>
+      <c r="F3" s="15">
         <v>43978</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="18">
+      <c r="G3" s="16"/>
+      <c r="H3" s="15">
         <v>43979</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="18">
+      <c r="I3" s="16"/>
+      <c r="J3" s="15">
         <v>43980</v>
       </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="18">
+      <c r="K3" s="16"/>
+      <c r="L3" s="15">
         <v>43983</v>
       </c>
-      <c r="M3" s="19"/>
-      <c r="N3" s="18">
+      <c r="M3" s="16"/>
+      <c r="N3" s="15">
         <v>43984</v>
       </c>
-      <c r="O3" s="19"/>
-      <c r="P3" s="18">
+      <c r="O3" s="16"/>
+      <c r="P3" s="15">
         <v>43985</v>
       </c>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="18">
+      <c r="Q3" s="16"/>
+      <c r="R3" s="15">
         <v>43986</v>
       </c>
-      <c r="S3" s="19"/>
-      <c r="T3" s="18">
+      <c r="S3" s="16"/>
+      <c r="T3" s="15">
         <v>43987</v>
       </c>
-      <c r="U3" s="19"/>
-      <c r="V3" s="18">
+      <c r="U3" s="16"/>
+      <c r="V3" s="15">
         <v>43990</v>
       </c>
-      <c r="W3" s="19"/>
-      <c r="X3" s="18">
+      <c r="W3" s="16"/>
+      <c r="X3" s="15">
         <v>43991</v>
       </c>
-      <c r="Y3" s="19"/>
+      <c r="Y3" s="16"/>
     </row>
     <row r="4" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -861,161 +861,161 @@
       <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="5"/>
     </row>
     <row r="8" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="5"/>
       <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="14"/>
       <c r="C13" s="8"/>
     </row>
     <row r="14" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="14"/>
       <c r="C15" s="8"/>
     </row>
     <row r="16" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="14"/>
       <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="14" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="14"/>
       <c r="D19" s="13"/>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="14"/>
       <c r="D21" s="13"/>
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="14" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
+      <c r="A23" s="14"/>
       <c r="D23" s="13"/>
     </row>
     <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="14"/>
       <c r="D25" s="13"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
+      <c r="A27" s="14"/>
       <c r="D27" s="13"/>
     </row>
     <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="14" t="s">
         <v>28</v>
       </c>
       <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
+      <c r="A29" s="14"/>
       <c r="D29" s="13"/>
     </row>
     <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="14" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
+      <c r="A31" s="14"/>
       <c r="E31" s="8"/>
     </row>
     <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
+      <c r="A33" s="14"/>
       <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="14" t="s">
         <v>39</v>
       </c>
       <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
+      <c r="A35" s="14"/>
       <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="14" t="s">
         <v>29</v>
       </c>
       <c r="F36" s="9"/>
@@ -1026,13 +1026,15 @@
       <c r="K36" s="7"/>
     </row>
     <row r="37" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
+      <c r="A37" s="14"/>
       <c r="E37" s="12"/>
       <c r="F37" s="13"/>
       <c r="G37" s="8"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="8"/>
     </row>
     <row r="38" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="14" t="s">
         <v>30</v>
       </c>
       <c r="J38" s="11"/>
@@ -1042,37 +1044,37 @@
       <c r="N38" s="9"/>
     </row>
     <row r="39" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
+      <c r="A39" s="14"/>
     </row>
     <row r="40" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="14" t="s">
         <v>31</v>
       </c>
       <c r="O40" s="7"/>
     </row>
     <row r="41" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
+      <c r="A41" s="14"/>
     </row>
     <row r="42" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="14" t="s">
         <v>32</v>
       </c>
       <c r="O42" s="7"/>
     </row>
     <row r="43" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
+      <c r="A43" s="14"/>
     </row>
     <row r="44" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="14" t="s">
         <v>33</v>
       </c>
       <c r="O44" s="7"/>
     </row>
     <row r="45" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
+      <c r="A45" s="14"/>
     </row>
     <row r="46" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="14" t="s">
         <v>34</v>
       </c>
       <c r="P46" s="9"/>
@@ -1080,10 +1082,10 @@
       <c r="R46" s="11"/>
     </row>
     <row r="47" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
+      <c r="A47" s="14"/>
     </row>
     <row r="48" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
+      <c r="A48" s="14" t="s">
         <v>35</v>
       </c>
       <c r="R48" s="11"/>
@@ -1096,10 +1098,10 @@
       <c r="Y48" s="7"/>
     </row>
     <row r="49" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
+      <c r="A49" s="14"/>
     </row>
     <row r="50" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
+      <c r="A50" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B50" s="2"/>
@@ -1128,16 +1130,18 @@
       <c r="Y50" s="7"/>
     </row>
     <row r="51" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
+      <c r="A51" s="14"/>
       <c r="B51" s="5"/>
       <c r="C51" s="8"/>
       <c r="D51" s="13"/>
       <c r="E51" s="8"/>
       <c r="F51" s="13"/>
       <c r="G51" s="8"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="8"/>
     </row>
     <row r="52" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="14" t="s">
         <v>37</v>
       </c>
       <c r="B52" s="2"/>
@@ -1166,41 +1170,83 @@
       <c r="Y52" s="7"/>
     </row>
     <row r="53" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
+      <c r="A53" s="14"/>
       <c r="B53" s="5"/>
       <c r="C53" s="8"/>
       <c r="D53" s="13"/>
       <c r="E53" s="8"/>
       <c r="F53" s="13"/>
       <c r="G53" s="8"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="8"/>
     </row>
     <row r="54" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
+      <c r="A54" s="14"/>
     </row>
     <row r="55" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
+      <c r="A55" s="14"/>
     </row>
     <row r="56" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
+      <c r="A56" s="14"/>
     </row>
     <row r="57" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
+      <c r="A57" s="14"/>
     </row>
     <row r="58" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
+      <c r="A58" s="14"/>
     </row>
     <row r="59" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
+      <c r="A59" s="14"/>
     </row>
     <row r="60" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="16"/>
+      <c r="A60" s="14"/>
     </row>
     <row r="61" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="16"/>
+      <c r="A61" s="14"/>
     </row>
     <row r="62" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="L1:Y1"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A28:A29"/>
     <mergeCell ref="A60:A61"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A18:A19"/>
@@ -1217,46 +1263,6 @@
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="L1:Y1"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modification Doc et algo
</commit_message>
<xml_diff>
--- a/Planning_CVRP.xlsx
+++ b/Planning_CVRP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Programming\C#\TPI\git\CVRP_Viewer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EF4995-8A66-417F-8ACE-E971378739F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8C20D5-D8C3-4B67-BE09-F3E3C1786FE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C268FC12-0260-4BE3-B295-C69B9861881F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Tâches</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>J11</t>
-  </si>
-  <si>
-    <t>J12</t>
   </si>
   <si>
     <t>Mai</t>
@@ -217,7 +214,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -287,11 +284,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -332,9 +338,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -344,13 +356,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -677,13 +689,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53423074-F718-4785-B7DE-E8325D9D0127}">
-  <dimension ref="A1:Y62"/>
+  <dimension ref="A1:Z62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q39" sqref="Q39"/>
+      <selection pane="bottomRight" activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,312 +723,303 @@
     <col min="21" max="21" width="3.7109375" style="3" customWidth="1"/>
     <col min="22" max="22" width="3.7109375" style="4" customWidth="1"/>
     <col min="23" max="23" width="3.7109375" style="3" customWidth="1"/>
-    <col min="24" max="24" width="3.7109375" style="4" customWidth="1"/>
-    <col min="25" max="25" width="3.7109375" style="3" customWidth="1"/>
-    <col min="26" max="16384" width="11.42578125" style="1"/>
+    <col min="24" max="26" width="11.42578125" style="4" customWidth="1"/>
+    <col min="27" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18" t="s">
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="F2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="21"/>
+      <c r="L2" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="21"/>
+      <c r="N2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="21"/>
+      <c r="P2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="21"/>
+      <c r="T2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="21"/>
+      <c r="V2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="W2" s="21"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="17">
+        <v>43976</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="17">
+        <v>43977</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="17">
+        <v>43978</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="17">
+        <v>43979</v>
+      </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="17">
+        <v>43980</v>
+      </c>
+      <c r="K3" s="18"/>
+      <c r="L3" s="17">
+        <v>43984</v>
+      </c>
+      <c r="M3" s="18"/>
+      <c r="N3" s="17">
+        <v>43985</v>
+      </c>
+      <c r="O3" s="18"/>
+      <c r="P3" s="17">
+        <v>43986</v>
+      </c>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="17">
+        <v>43987</v>
+      </c>
+      <c r="S3" s="18"/>
+      <c r="T3" s="17">
+        <v>43990</v>
+      </c>
+      <c r="U3" s="18"/>
+      <c r="V3" s="17">
+        <v>43991</v>
+      </c>
+      <c r="W3" s="18"/>
+    </row>
+    <row r="4" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="S2" s="20"/>
-      <c r="T2" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="U2" s="20"/>
-      <c r="V2" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="W2" s="20"/>
-      <c r="X2" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y2" s="20"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="15">
-        <v>43976</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="15">
-        <v>43977</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="15">
-        <v>43978</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="15">
-        <v>43979</v>
-      </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="15">
-        <v>43980</v>
-      </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="15">
-        <v>43983</v>
-      </c>
-      <c r="M3" s="16"/>
-      <c r="N3" s="15">
-        <v>43984</v>
-      </c>
-      <c r="O3" s="16"/>
-      <c r="P3" s="15">
-        <v>43985</v>
-      </c>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="15">
-        <v>43986</v>
-      </c>
-      <c r="S3" s="16"/>
-      <c r="T3" s="15">
-        <v>43987</v>
-      </c>
-      <c r="U3" s="16"/>
-      <c r="V3" s="15">
-        <v>43990</v>
-      </c>
-      <c r="W3" s="16"/>
-      <c r="X3" s="15">
-        <v>43991</v>
-      </c>
-      <c r="Y3" s="16"/>
-    </row>
-    <row r="4" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>18</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="5"/>
       <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="D19" s="13"/>
+    </row>
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="D19" s="13"/>
-    </row>
-    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="D23" s="13"/>
+    </row>
+    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>24</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="15"/>
       <c r="D25" s="13"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="D27" s="13"/>
-    </row>
-    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="F35" s="13"/>
+    </row>
+    <row r="36" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
         <v>28</v>
-      </c>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="D29" s="13"/>
-    </row>
-    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="F35" s="13"/>
-    </row>
-    <row r="36" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>29</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="7"/>
@@ -1026,7 +1029,7 @@
       <c r="K36" s="7"/>
     </row>
     <row r="37" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+      <c r="A37" s="15"/>
       <c r="E37" s="12"/>
       <c r="F37" s="13"/>
       <c r="G37" s="8"/>
@@ -1034,8 +1037,8 @@
       <c r="I37" s="8"/>
     </row>
     <row r="38" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
-        <v>30</v>
+      <c r="A38" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="J38" s="11"/>
       <c r="K38" s="12"/>
@@ -1044,65 +1047,71 @@
       <c r="N38" s="9"/>
     </row>
     <row r="39" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="15"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="8"/>
     </row>
     <row r="40" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="O40" s="7"/>
+    </row>
+    <row r="41" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="15"/>
+    </row>
+    <row r="42" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="O40" s="7"/>
-    </row>
-    <row r="41" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-    </row>
-    <row r="42" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="s">
+      <c r="O42" s="7"/>
+    </row>
+    <row r="43" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="15"/>
+    </row>
+    <row r="44" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="O42" s="7"/>
-    </row>
-    <row r="43" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
-    </row>
-    <row r="44" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
+      <c r="O44" s="7"/>
+    </row>
+    <row r="45" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="15"/>
+    </row>
+    <row r="46" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="O44" s="7"/>
-    </row>
-    <row r="45" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
-    </row>
-    <row r="46" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
-        <v>34</v>
       </c>
       <c r="P46" s="9"/>
       <c r="Q46" s="7"/>
       <c r="R46" s="11"/>
     </row>
     <row r="47" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="A47" s="15"/>
     </row>
     <row r="48" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
-        <v>35</v>
+      <c r="A48" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="R48" s="11"/>
       <c r="S48" s="12"/>
-      <c r="T48" s="11"/>
-      <c r="U48" s="12"/>
+      <c r="T48" s="9"/>
+      <c r="U48" s="7"/>
       <c r="V48" s="9"/>
       <c r="W48" s="7"/>
-      <c r="X48" s="9"/>
-      <c r="Y48" s="7"/>
+      <c r="X48" s="11"/>
+      <c r="Y48" s="11"/>
     </row>
     <row r="49" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="A49" s="15"/>
+      <c r="X49" s="11"/>
+      <c r="Y49" s="11"/>
     </row>
     <row r="50" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
-        <v>36</v>
+      <c r="A50" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="7"/>
@@ -1126,11 +1135,11 @@
       <c r="U50" s="7"/>
       <c r="V50" s="9"/>
       <c r="W50" s="7"/>
-      <c r="X50" s="9"/>
-      <c r="Y50" s="7"/>
+      <c r="X50" s="11"/>
+      <c r="Y50" s="11"/>
     </row>
     <row r="51" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="5"/>
       <c r="C51" s="8"/>
       <c r="D51" s="13"/>
@@ -1139,10 +1148,16 @@
       <c r="G51" s="8"/>
       <c r="H51" s="13"/>
       <c r="I51" s="8"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="8"/>
+      <c r="X51" s="11"/>
+      <c r="Y51" s="11"/>
     </row>
     <row r="52" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
-        <v>37</v>
+      <c r="A52" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="7"/>
@@ -1166,11 +1181,11 @@
       <c r="U52" s="7"/>
       <c r="V52" s="9"/>
       <c r="W52" s="7"/>
-      <c r="X52" s="9"/>
-      <c r="Y52" s="7"/>
+      <c r="X52" s="11"/>
+      <c r="Y52" s="11"/>
     </row>
     <row r="53" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="5"/>
       <c r="C53" s="8"/>
       <c r="D53" s="13"/>
@@ -1179,55 +1194,43 @@
       <c r="G53" s="8"/>
       <c r="H53" s="13"/>
       <c r="I53" s="8"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="8"/>
     </row>
     <row r="54" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
+      <c r="A54" s="15"/>
     </row>
     <row r="55" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
+      <c r="A55" s="15"/>
     </row>
     <row r="56" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
+      <c r="A56" s="15"/>
     </row>
     <row r="57" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="15"/>
     </row>
     <row r="58" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
+      <c r="A58" s="15"/>
     </row>
     <row r="59" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="15"/>
     </row>
     <row r="60" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
+      <c r="A60" s="15"/>
     </row>
     <row r="61" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
+      <c r="A61" s="15"/>
     </row>
     <row r="62" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A26:A27"/>
+  <mergeCells count="54">
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="L1:Y1"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="N2:O2"/>
@@ -1235,6 +1238,18 @@
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A30:A31"/>
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="N3:O3"/>
@@ -1242,10 +1257,15 @@
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="L1:W1"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A60:A61"/>
     <mergeCell ref="A24:A25"/>
@@ -1260,9 +1280,6 @@
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Algorithme fonctionne avec 3, 2 et 1 nodes
</commit_message>
<xml_diff>
--- a/Planning_CVRP.xlsx
+++ b/Planning_CVRP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Programming\C#\TPI\git\CVRP_Viewer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8C20D5-D8C3-4B67-BE09-F3E3C1786FE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDADBE4-0BBD-48C1-8E9F-6AC9981541A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C268FC12-0260-4BE3-B295-C69B9861881F}"/>
   </bookViews>
@@ -344,29 +344,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -695,7 +695,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M53" sqref="M53"/>
+      <selection pane="bottomRight" activeCell="Z46" sqref="Z46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,139 +728,139 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="16" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="20" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="20" t="s">
+      <c r="I2" s="19"/>
+      <c r="J2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="20" t="s">
+      <c r="K2" s="19"/>
+      <c r="L2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="21"/>
-      <c r="N2" s="20" t="s">
+      <c r="M2" s="19"/>
+      <c r="N2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="20" t="s">
+      <c r="O2" s="19"/>
+      <c r="P2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="20" t="s">
+      <c r="Q2" s="19"/>
+      <c r="R2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="21"/>
-      <c r="T2" s="20" t="s">
+      <c r="S2" s="19"/>
+      <c r="T2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="21"/>
-      <c r="V2" s="20" t="s">
+      <c r="U2" s="19"/>
+      <c r="V2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="21"/>
+      <c r="W2" s="19"/>
       <c r="X2" s="14"/>
       <c r="Y2" s="14"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="17">
+      <c r="A3" s="21"/>
+      <c r="B3" s="16">
         <v>43976</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="17">
+      <c r="C3" s="17"/>
+      <c r="D3" s="16">
         <v>43977</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="17">
+      <c r="E3" s="17"/>
+      <c r="F3" s="16">
         <v>43978</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="17">
+      <c r="G3" s="17"/>
+      <c r="H3" s="16">
         <v>43979</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="17">
+      <c r="I3" s="17"/>
+      <c r="J3" s="16">
         <v>43980</v>
       </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="17">
+      <c r="K3" s="17"/>
+      <c r="L3" s="16">
         <v>43984</v>
       </c>
-      <c r="M3" s="18"/>
-      <c r="N3" s="17">
+      <c r="M3" s="17"/>
+      <c r="N3" s="16">
         <v>43985</v>
       </c>
-      <c r="O3" s="18"/>
-      <c r="P3" s="17">
+      <c r="O3" s="17"/>
+      <c r="P3" s="16">
         <v>43986</v>
       </c>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="17">
+      <c r="Q3" s="17"/>
+      <c r="R3" s="16">
         <v>43987</v>
       </c>
-      <c r="S3" s="18"/>
-      <c r="T3" s="17">
+      <c r="S3" s="17"/>
+      <c r="T3" s="16">
         <v>43990</v>
       </c>
-      <c r="U3" s="18"/>
-      <c r="V3" s="17">
+      <c r="U3" s="17"/>
+      <c r="V3" s="16">
         <v>43991</v>
       </c>
-      <c r="W3" s="18"/>
+      <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1052,6 +1052,7 @@
       <c r="K39" s="8"/>
       <c r="L39" s="13"/>
       <c r="M39" s="8"/>
+      <c r="N39" s="13"/>
     </row>
     <row r="40" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
@@ -1152,6 +1153,7 @@
       <c r="K51" s="8"/>
       <c r="L51" s="13"/>
       <c r="M51" s="8"/>
+      <c r="N51" s="13"/>
       <c r="X51" s="11"/>
       <c r="Y51" s="11"/>
     </row>
@@ -1198,6 +1200,7 @@
       <c r="K53" s="8"/>
       <c r="L53" s="13"/>
       <c r="M53" s="8"/>
+      <c r="N53" s="13"/>
     </row>
     <row r="54" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
@@ -1226,28 +1229,22 @@
     <row r="62" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="L1:W1"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="R3:S3"/>
@@ -1264,22 +1261,28 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="L1:W1"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nettoyage du code et explication du programme dans doc
</commit_message>
<xml_diff>
--- a/Planning_CVRP.xlsx
+++ b/Planning_CVRP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Programming\C#\TPI\git\CVRP_Viewer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDADBE4-0BBD-48C1-8E9F-6AC9981541A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEEAED9-2917-4381-AAC7-9B80D1C35FFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C268FC12-0260-4BE3-B295-C69B9861881F}"/>
   </bookViews>
@@ -344,28 +344,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -692,10 +692,10 @@
   <dimension ref="A1:Z62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Z46" sqref="Z46"/>
+      <selection pane="bottomRight" activeCell="R45" sqref="R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,130 +728,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="23" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="18" t="s">
+      <c r="G2" s="21"/>
+      <c r="H2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="18" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="18" t="s">
+      <c r="K2" s="21"/>
+      <c r="L2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="19"/>
-      <c r="N2" s="18" t="s">
+      <c r="M2" s="21"/>
+      <c r="N2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="19"/>
-      <c r="P2" s="18" t="s">
+      <c r="O2" s="21"/>
+      <c r="P2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="18" t="s">
+      <c r="Q2" s="21"/>
+      <c r="R2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="19"/>
-      <c r="T2" s="18" t="s">
+      <c r="S2" s="21"/>
+      <c r="T2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="19"/>
-      <c r="V2" s="18" t="s">
+      <c r="U2" s="21"/>
+      <c r="V2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="19"/>
+      <c r="W2" s="21"/>
       <c r="X2" s="14"/>
       <c r="Y2" s="14"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="16">
+      <c r="A3" s="19"/>
+      <c r="B3" s="17">
         <v>43976</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="16">
+      <c r="C3" s="18"/>
+      <c r="D3" s="17">
         <v>43977</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="16">
+      <c r="E3" s="18"/>
+      <c r="F3" s="17">
         <v>43978</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="16">
+      <c r="G3" s="18"/>
+      <c r="H3" s="17">
         <v>43979</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="16">
+      <c r="I3" s="18"/>
+      <c r="J3" s="17">
         <v>43980</v>
       </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="16">
+      <c r="K3" s="18"/>
+      <c r="L3" s="17">
         <v>43984</v>
       </c>
-      <c r="M3" s="17"/>
-      <c r="N3" s="16">
+      <c r="M3" s="18"/>
+      <c r="N3" s="17">
         <v>43985</v>
       </c>
-      <c r="O3" s="17"/>
-      <c r="P3" s="16">
+      <c r="O3" s="18"/>
+      <c r="P3" s="17">
         <v>43986</v>
       </c>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="16">
+      <c r="Q3" s="18"/>
+      <c r="R3" s="17">
         <v>43987</v>
       </c>
-      <c r="S3" s="17"/>
-      <c r="T3" s="16">
+      <c r="S3" s="18"/>
+      <c r="T3" s="17">
         <v>43990</v>
       </c>
-      <c r="U3" s="17"/>
-      <c r="V3" s="16">
+      <c r="U3" s="18"/>
+      <c r="V3" s="17">
         <v>43991</v>
       </c>
-      <c r="W3" s="17"/>
+      <c r="W3" s="18"/>
     </row>
     <row r="4" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
@@ -1062,6 +1062,7 @@
     </row>
     <row r="41" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
+      <c r="O41" s="8"/>
     </row>
     <row r="42" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
@@ -1071,6 +1072,7 @@
     </row>
     <row r="43" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
+      <c r="O43" s="8"/>
     </row>
     <row r="44" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
@@ -1080,6 +1082,7 @@
     </row>
     <row r="45" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
+      <c r="O45" s="8"/>
     </row>
     <row r="46" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
@@ -1154,6 +1157,7 @@
       <c r="L51" s="13"/>
       <c r="M51" s="8"/>
       <c r="N51" s="13"/>
+      <c r="O51" s="8"/>
       <c r="X51" s="11"/>
       <c r="Y51" s="11"/>
     </row>
@@ -1201,6 +1205,7 @@
       <c r="L53" s="13"/>
       <c r="M53" s="8"/>
       <c r="N53" s="13"/>
+      <c r="O53" s="8"/>
     </row>
     <row r="54" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
@@ -1229,6 +1234,44 @@
     <row r="62" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A26:A27"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="L1:W1"/>
     <mergeCell ref="A28:A29"/>
@@ -1245,44 +1288,6 @@
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout des tests et btnChooseFile dans doc
</commit_message>
<xml_diff>
--- a/Planning_CVRP.xlsx
+++ b/Planning_CVRP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Programming\C#\TPI\git\CVRP_Viewer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D13A36-967D-40E7-9FFC-A1A389592357}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F1993A-8FF4-46A2-BBF6-B9D38DD140F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C268FC12-0260-4BE3-B295-C69B9861881F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Tâches</t>
   </si>
@@ -695,10 +695,10 @@
   <dimension ref="A1:Z62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q55" sqref="Q55"/>
+      <selection pane="bottomRight" activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,6 +1099,7 @@
       <c r="A47" s="15"/>
       <c r="P47" s="13"/>
       <c r="Q47" s="8"/>
+      <c r="S47" s="8"/>
     </row>
     <row r="48" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
@@ -1115,6 +1116,8 @@
     </row>
     <row r="49" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="13"/>
       <c r="X49" s="11"/>
       <c r="Y49" s="11"/>
     </row>
@@ -1123,41 +1126,26 @@
         <v>34</v>
       </c>
       <c r="R50" s="11"/>
-      <c r="S50" s="12"/>
-      <c r="T50" s="9"/>
-      <c r="U50" s="7"/>
-      <c r="V50" s="9"/>
-      <c r="W50" s="7"/>
+      <c r="S50" s="7"/>
+      <c r="T50" s="11"/>
+      <c r="U50" s="12"/>
+      <c r="V50" s="11"/>
+      <c r="W50" s="12"/>
       <c r="X50" s="11"/>
       <c r="Y50" s="11"/>
     </row>
     <row r="51" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="15"/>
+      <c r="S51" s="8"/>
       <c r="X51" s="11"/>
       <c r="Y51" s="11"/>
     </row>
     <row r="52" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="9"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="9"/>
-      <c r="O52" s="7"/>
-      <c r="P52" s="9"/>
-      <c r="Q52" s="7"/>
-      <c r="R52" s="9"/>
-      <c r="S52" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="R52" s="11"/>
+      <c r="S52" s="12"/>
       <c r="T52" s="9"/>
       <c r="U52" s="7"/>
       <c r="V52" s="9"/>
@@ -1167,26 +1155,10 @@
     </row>
     <row r="53" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="15"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="8"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="8"/>
-      <c r="L53" s="13"/>
-      <c r="M53" s="8"/>
-      <c r="N53" s="13"/>
-      <c r="O53" s="8"/>
-      <c r="P53" s="13"/>
-      <c r="Q53" s="8"/>
     </row>
     <row r="54" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="7"/>
@@ -1229,12 +1201,56 @@
       <c r="O55" s="8"/>
       <c r="P55" s="13"/>
       <c r="Q55" s="8"/>
+      <c r="R55" s="13"/>
+      <c r="S55" s="8"/>
     </row>
     <row r="56" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
+      <c r="A56" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="9"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="9"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="9"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="9"/>
+      <c r="U56" s="7"/>
+      <c r="V56" s="9"/>
+      <c r="W56" s="7"/>
     </row>
     <row r="57" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="15"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="8"/>
+      <c r="N57" s="13"/>
+      <c r="O57" s="8"/>
+      <c r="P57" s="13"/>
+      <c r="Q57" s="8"/>
+      <c r="R57" s="13"/>
+      <c r="S57" s="8"/>
     </row>
     <row r="58" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>

</xml_diff>

<commit_message>
Création du Résumé du rapport TPI et avencement sur la conclusion de la doc
</commit_message>
<xml_diff>
--- a/Planning_CVRP.xlsx
+++ b/Planning_CVRP.xlsx
@@ -8,13 +8,56 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Programming\C#\TPI\git\CVRP_Viewer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F1993A-8FF4-46A2-BBF6-B9D38DD140F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD39A57-B73D-4B60-8D0F-41C36487C1DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C268FC12-0260-4BE3-B295-C69B9861881F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v5.0" hidden="1">Planning!$H$47</definedName>
+    <definedName name="_xlchart.v5.1" hidden="1">Planning!$H$48</definedName>
+    <definedName name="_xlchart.v5.10" hidden="1">Planning!$I$50</definedName>
+    <definedName name="_xlchart.v5.11" hidden="1">Planning!$I$51</definedName>
+    <definedName name="_xlchart.v5.12" hidden="1">Planning!$I$52</definedName>
+    <definedName name="_xlchart.v5.13" hidden="1">Planning!$J$46:$Q$46</definedName>
+    <definedName name="_xlchart.v5.14" hidden="1">Planning!$J$47:$Q$47</definedName>
+    <definedName name="_xlchart.v5.15" hidden="1">Planning!$J$48:$Q$48</definedName>
+    <definedName name="_xlchart.v5.16" hidden="1">Planning!$J$49:$Q$49</definedName>
+    <definedName name="_xlchart.v5.17" hidden="1">Planning!$J$50:$Q$50</definedName>
+    <definedName name="_xlchart.v5.18" hidden="1">Planning!$J$51:$Q$51</definedName>
+    <definedName name="_xlchart.v5.19" hidden="1">Planning!$J$52:$Q$52</definedName>
+    <definedName name="_xlchart.v5.2" hidden="1">Planning!$H$49</definedName>
+    <definedName name="_xlchart.v5.20" hidden="1">Planning!$O$47</definedName>
+    <definedName name="_xlchart.v5.21" hidden="1">Planning!$P$46</definedName>
+    <definedName name="_xlchart.v5.22" hidden="1">Planning!$P$47</definedName>
+    <definedName name="_xlchart.v5.23" hidden="1">Planning!$Q$46</definedName>
+    <definedName name="_xlchart.v5.24" hidden="1">Planning!$Q$47</definedName>
+    <definedName name="_xlchart.v5.25" hidden="1">Planning!$Y$46</definedName>
+    <definedName name="_xlchart.v5.26" hidden="1">Planning!$Y$47</definedName>
+    <definedName name="_xlchart.v5.27" hidden="1">Planning!$Z$46</definedName>
+    <definedName name="_xlchart.v5.28" hidden="1">Planning!$Z$47</definedName>
+    <definedName name="_xlchart.v5.29" hidden="1">Planning!$X$47</definedName>
+    <definedName name="_xlchart.v5.3" hidden="1">Planning!$H$50</definedName>
+    <definedName name="_xlchart.v5.30" hidden="1">Planning!$Y$47</definedName>
+    <definedName name="_xlchart.v5.31" hidden="1">Planning!$Y$46</definedName>
+    <definedName name="_xlchart.v5.32" hidden="1">Planning!$Y$47</definedName>
+    <definedName name="_xlchart.v5.33" hidden="1">Planning!$Y$47:$Y$48</definedName>
+    <definedName name="_xlchart.v5.34" hidden="1">Planning!$Y$47:$Y$49</definedName>
+    <definedName name="_xlchart.v5.35" hidden="1">Planning!$Y$47:$Y$50</definedName>
+    <definedName name="_xlchart.v5.36" hidden="1">Planning!$Z$46</definedName>
+    <definedName name="_xlchart.v5.37" hidden="1">Planning!$Z$47</definedName>
+    <definedName name="_xlchart.v5.38" hidden="1">Planning!$Z$47:$Z$48</definedName>
+    <definedName name="_xlchart.v5.39" hidden="1">Planning!$Z$47:$Z$49</definedName>
+    <definedName name="_xlchart.v5.4" hidden="1">Planning!$H$51</definedName>
+    <definedName name="_xlchart.v5.40" hidden="1">Planning!$Z$47:$Z$50</definedName>
+    <definedName name="_xlchart.v5.5" hidden="1">Planning!$H$52</definedName>
+    <definedName name="_xlchart.v5.6" hidden="1">Planning!$I$46</definedName>
+    <definedName name="_xlchart.v5.7" hidden="1">Planning!$I$47</definedName>
+    <definedName name="_xlchart.v5.8" hidden="1">Planning!$I$48</definedName>
+    <definedName name="_xlchart.v5.9" hidden="1">Planning!$I$49</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Tâches</t>
   </si>
@@ -137,9 +180,6 @@
     <t>Manuel utilisateur</t>
   </si>
   <si>
-    <t>Résumé du TPI</t>
-  </si>
-  <si>
     <t>Journal de tavail</t>
   </si>
   <si>
@@ -153,6 +193,9 @@
   </si>
   <si>
     <t>Nettoyage du code</t>
+  </si>
+  <si>
+    <t>Rapport TPI</t>
   </si>
 </sst>
 </file>
@@ -300,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -347,29 +390,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -695,10 +744,10 @@
   <dimension ref="A1:Z62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O37" sqref="O37"/>
+      <selection pane="bottomRight" activeCell="A52" sqref="A52:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,130 +780,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="23" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="18" t="s">
+      <c r="G2" s="21"/>
+      <c r="H2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="18" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="18" t="s">
+      <c r="K2" s="21"/>
+      <c r="L2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="19"/>
-      <c r="N2" s="18" t="s">
+      <c r="M2" s="21"/>
+      <c r="N2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="19"/>
-      <c r="P2" s="18" t="s">
+      <c r="O2" s="21"/>
+      <c r="P2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="18" t="s">
+      <c r="Q2" s="21"/>
+      <c r="R2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="19"/>
-      <c r="T2" s="18" t="s">
+      <c r="S2" s="21"/>
+      <c r="T2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="19"/>
-      <c r="V2" s="18" t="s">
+      <c r="U2" s="21"/>
+      <c r="V2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="19"/>
+      <c r="W2" s="21"/>
       <c r="X2" s="14"/>
       <c r="Y2" s="14"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="16">
+      <c r="A3" s="19"/>
+      <c r="B3" s="17">
         <v>43976</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="16">
+      <c r="C3" s="18"/>
+      <c r="D3" s="17">
         <v>43977</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="16">
+      <c r="E3" s="18"/>
+      <c r="F3" s="17">
         <v>43978</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="16">
+      <c r="G3" s="18"/>
+      <c r="H3" s="17">
         <v>43979</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="16">
+      <c r="I3" s="18"/>
+      <c r="J3" s="17">
         <v>43980</v>
       </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="16">
+      <c r="K3" s="18"/>
+      <c r="L3" s="17">
         <v>43984</v>
       </c>
-      <c r="M3" s="17"/>
-      <c r="N3" s="16">
+      <c r="M3" s="18"/>
+      <c r="N3" s="17">
         <v>43985</v>
       </c>
-      <c r="O3" s="17"/>
-      <c r="P3" s="16">
+      <c r="O3" s="18"/>
+      <c r="P3" s="17">
         <v>43986</v>
       </c>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="16">
+      <c r="Q3" s="18"/>
+      <c r="R3" s="17">
         <v>43987</v>
       </c>
-      <c r="S3" s="17"/>
-      <c r="T3" s="16">
+      <c r="S3" s="18"/>
+      <c r="T3" s="17">
         <v>43990</v>
       </c>
-      <c r="U3" s="17"/>
-      <c r="V3" s="16">
+      <c r="U3" s="18"/>
+      <c r="V3" s="17">
         <v>43991</v>
       </c>
-      <c r="W3" s="17"/>
+      <c r="W3" s="18"/>
     </row>
     <row r="4" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
@@ -972,7 +1021,7 @@
     </row>
     <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" s="9"/>
     </row>
@@ -1012,7 +1061,7 @@
     </row>
     <row r="34" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F34" s="9"/>
     </row>
@@ -1103,7 +1152,7 @@
     </row>
     <row r="48" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R48" s="9"/>
       <c r="S48" s="7"/>
@@ -1123,20 +1172,21 @@
     </row>
     <row r="50" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="R50" s="11"/>
-      <c r="S50" s="7"/>
-      <c r="T50" s="11"/>
-      <c r="U50" s="12"/>
-      <c r="V50" s="11"/>
-      <c r="W50" s="12"/>
+      <c r="S50" s="12"/>
+      <c r="T50" s="9"/>
+      <c r="U50" s="7"/>
+      <c r="V50" s="9"/>
+      <c r="W50" s="7"/>
       <c r="X50" s="11"/>
       <c r="Y50" s="11"/>
     </row>
     <row r="51" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="15"/>
-      <c r="S51" s="8"/>
+      <c r="T51" s="13"/>
+      <c r="U51" s="8"/>
       <c r="X51" s="11"/>
       <c r="Y51" s="11"/>
     </row>
@@ -1144,8 +1194,24 @@
       <c r="A52" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="R52" s="11"/>
-      <c r="S52" s="12"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="7"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="7"/>
+      <c r="N52" s="9"/>
+      <c r="O52" s="7"/>
+      <c r="P52" s="9"/>
+      <c r="Q52" s="7"/>
+      <c r="R52" s="9"/>
+      <c r="S52" s="7"/>
       <c r="T52" s="9"/>
       <c r="U52" s="7"/>
       <c r="V52" s="9"/>
@@ -1155,6 +1221,26 @@
     </row>
     <row r="53" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="15"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="13"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="13"/>
+      <c r="Q53" s="8"/>
+      <c r="R53" s="13"/>
+      <c r="S53" s="8"/>
+      <c r="T53" s="13"/>
+      <c r="U53" s="8"/>
     </row>
     <row r="54" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
@@ -1203,54 +1289,58 @@
       <c r="Q55" s="8"/>
       <c r="R55" s="13"/>
       <c r="S55" s="8"/>
+      <c r="T55" s="13"/>
+      <c r="U55" s="8"/>
     </row>
     <row r="56" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="9"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="9"/>
-      <c r="M56" s="7"/>
-      <c r="N56" s="9"/>
-      <c r="O56" s="7"/>
-      <c r="P56" s="9"/>
-      <c r="Q56" s="7"/>
-      <c r="R56" s="9"/>
-      <c r="S56" s="7"/>
-      <c r="T56" s="9"/>
-      <c r="U56" s="7"/>
-      <c r="V56" s="9"/>
-      <c r="W56" s="7"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="12"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="12"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="12"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="12"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="12"/>
+      <c r="T56" s="11"/>
+      <c r="U56" s="12"/>
+      <c r="V56" s="11"/>
+      <c r="W56" s="12"/>
     </row>
     <row r="57" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="13"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="13"/>
-      <c r="M57" s="8"/>
-      <c r="N57" s="13"/>
-      <c r="O57" s="8"/>
-      <c r="P57" s="13"/>
-      <c r="Q57" s="8"/>
-      <c r="R57" s="13"/>
-      <c r="S57" s="8"/>
+      <c r="A57" s="24"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="12"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="12"/>
+      <c r="N57" s="11"/>
+      <c r="O57" s="12"/>
+      <c r="P57" s="11"/>
+      <c r="Q57" s="12"/>
+      <c r="R57" s="11"/>
+      <c r="S57" s="12"/>
+      <c r="T57" s="11"/>
+      <c r="U57" s="12"/>
+      <c r="V57" s="11"/>
+      <c r="W57" s="12"/>
     </row>
     <row r="58" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
@@ -1267,6 +1357,44 @@
     <row r="62" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A26:A27"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="L1:W1"/>
     <mergeCell ref="A28:A29"/>
@@ -1283,44 +1411,6 @@
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finalisation des documents à rendre
</commit_message>
<xml_diff>
--- a/Planning_CVRP.xlsx
+++ b/Planning_CVRP.xlsx
@@ -8,56 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Programming\C#\TPI\git\CVRP_Viewer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD39A57-B73D-4B60-8D0F-41C36487C1DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1375398-26CA-41A0-924D-556176D05D5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C268FC12-0260-4BE3-B295-C69B9861881F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v5.0" hidden="1">Planning!$H$47</definedName>
-    <definedName name="_xlchart.v5.1" hidden="1">Planning!$H$48</definedName>
-    <definedName name="_xlchart.v5.10" hidden="1">Planning!$I$50</definedName>
-    <definedName name="_xlchart.v5.11" hidden="1">Planning!$I$51</definedName>
-    <definedName name="_xlchart.v5.12" hidden="1">Planning!$I$52</definedName>
-    <definedName name="_xlchart.v5.13" hidden="1">Planning!$J$46:$Q$46</definedName>
-    <definedName name="_xlchart.v5.14" hidden="1">Planning!$J$47:$Q$47</definedName>
-    <definedName name="_xlchart.v5.15" hidden="1">Planning!$J$48:$Q$48</definedName>
-    <definedName name="_xlchart.v5.16" hidden="1">Planning!$J$49:$Q$49</definedName>
-    <definedName name="_xlchart.v5.17" hidden="1">Planning!$J$50:$Q$50</definedName>
-    <definedName name="_xlchart.v5.18" hidden="1">Planning!$J$51:$Q$51</definedName>
-    <definedName name="_xlchart.v5.19" hidden="1">Planning!$J$52:$Q$52</definedName>
-    <definedName name="_xlchart.v5.2" hidden="1">Planning!$H$49</definedName>
-    <definedName name="_xlchart.v5.20" hidden="1">Planning!$O$47</definedName>
-    <definedName name="_xlchart.v5.21" hidden="1">Planning!$P$46</definedName>
-    <definedName name="_xlchart.v5.22" hidden="1">Planning!$P$47</definedName>
-    <definedName name="_xlchart.v5.23" hidden="1">Planning!$Q$46</definedName>
-    <definedName name="_xlchart.v5.24" hidden="1">Planning!$Q$47</definedName>
-    <definedName name="_xlchart.v5.25" hidden="1">Planning!$Y$46</definedName>
-    <definedName name="_xlchart.v5.26" hidden="1">Planning!$Y$47</definedName>
-    <definedName name="_xlchart.v5.27" hidden="1">Planning!$Z$46</definedName>
-    <definedName name="_xlchart.v5.28" hidden="1">Planning!$Z$47</definedName>
-    <definedName name="_xlchart.v5.29" hidden="1">Planning!$X$47</definedName>
-    <definedName name="_xlchart.v5.3" hidden="1">Planning!$H$50</definedName>
-    <definedName name="_xlchart.v5.30" hidden="1">Planning!$Y$47</definedName>
-    <definedName name="_xlchart.v5.31" hidden="1">Planning!$Y$46</definedName>
-    <definedName name="_xlchart.v5.32" hidden="1">Planning!$Y$47</definedName>
-    <definedName name="_xlchart.v5.33" hidden="1">Planning!$Y$47:$Y$48</definedName>
-    <definedName name="_xlchart.v5.34" hidden="1">Planning!$Y$47:$Y$49</definedName>
-    <definedName name="_xlchart.v5.35" hidden="1">Planning!$Y$47:$Y$50</definedName>
-    <definedName name="_xlchart.v5.36" hidden="1">Planning!$Z$46</definedName>
-    <definedName name="_xlchart.v5.37" hidden="1">Planning!$Z$47</definedName>
-    <definedName name="_xlchart.v5.38" hidden="1">Planning!$Z$47:$Z$48</definedName>
-    <definedName name="_xlchart.v5.39" hidden="1">Planning!$Z$47:$Z$49</definedName>
-    <definedName name="_xlchart.v5.4" hidden="1">Planning!$H$51</definedName>
-    <definedName name="_xlchart.v5.40" hidden="1">Planning!$Z$47:$Z$50</definedName>
-    <definedName name="_xlchart.v5.5" hidden="1">Planning!$H$52</definedName>
-    <definedName name="_xlchart.v5.6" hidden="1">Planning!$I$46</definedName>
-    <definedName name="_xlchart.v5.7" hidden="1">Planning!$I$47</definedName>
-    <definedName name="_xlchart.v5.8" hidden="1">Planning!$I$48</definedName>
-    <definedName name="_xlchart.v5.9" hidden="1">Planning!$I$49</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -159,15 +116,6 @@
     <t>Création du parser des fichiers .dat</t>
   </si>
   <si>
-    <t>Écrire le test unitaire des calcules de distance</t>
-  </si>
-  <si>
-    <t>Trouver la solution optimal en déplacent un client à la fois</t>
-  </si>
-  <si>
-    <t>Trouver la solution optimal en déplacent trois client à la fois</t>
-  </si>
-  <si>
     <t>Afficher les tournées dans la console</t>
   </si>
   <si>
@@ -180,9 +128,6 @@
     <t>Manuel utilisateur</t>
   </si>
   <si>
-    <t>Journal de tavail</t>
-  </si>
-  <si>
     <t>Documentation Technique</t>
   </si>
   <si>
@@ -195,7 +140,19 @@
     <t>Nettoyage du code</t>
   </si>
   <si>
-    <t>Rapport TPI</t>
+    <t>Résumé du         rapport TPI</t>
+  </si>
+  <si>
+    <t>Trouver la solution optimale en déplace un client à la fois</t>
+  </si>
+  <si>
+    <t>Écrire le test unitaire des calculs de distance</t>
+  </si>
+  <si>
+    <t>Journal de travail</t>
+  </si>
+  <si>
+    <t>Trouver la solution optimale en déplace trois clients à la fois</t>
   </si>
 </sst>
 </file>
@@ -387,38 +344,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -744,10 +701,10 @@
   <dimension ref="A1:Z62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A52" sqref="A52:A53"/>
+      <selection pane="bottomRight" activeCell="A38" sqref="A38:A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,86 +737,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="16" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="20" t="s">
+      <c r="E2" s="20"/>
+      <c r="F2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="20"/>
+      <c r="H2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="20" t="s">
+      <c r="I2" s="20"/>
+      <c r="J2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="20" t="s">
+      <c r="K2" s="20"/>
+      <c r="L2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="21"/>
-      <c r="N2" s="20" t="s">
+      <c r="M2" s="20"/>
+      <c r="N2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="20" t="s">
+      <c r="O2" s="20"/>
+      <c r="P2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="20" t="s">
+      <c r="Q2" s="20"/>
+      <c r="R2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="21"/>
-      <c r="T2" s="20" t="s">
+      <c r="S2" s="20"/>
+      <c r="T2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="21"/>
-      <c r="V2" s="20" t="s">
+      <c r="U2" s="20"/>
+      <c r="V2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="21"/>
+      <c r="W2" s="20"/>
       <c r="X2" s="14"/>
       <c r="Y2" s="14"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="17">
         <v>43976</v>
       </c>
@@ -906,172 +863,172 @@
       <c r="W3" s="18"/>
     </row>
     <row r="4" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="5"/>
     </row>
     <row r="8" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="5"/>
       <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="A13" s="16"/>
       <c r="C13" s="8"/>
     </row>
     <row r="14" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="A15" s="16"/>
       <c r="C15" s="8"/>
     </row>
     <row r="16" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+      <c r="A17" s="16"/>
       <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="16" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+      <c r="A19" s="16"/>
       <c r="D19" s="13"/>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
+      <c r="A21" s="16"/>
       <c r="D21" s="13"/>
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
+      <c r="A23" s="16"/>
       <c r="D23" s="13"/>
     </row>
     <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
+      <c r="A25" s="16"/>
       <c r="D25" s="13"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="16"/>
+      <c r="F35" s="13"/>
+    </row>
+    <row r="36" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
         <v>36</v>
-      </c>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="D27" s="13"/>
-    </row>
-    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="D29" s="13"/>
-    </row>
-    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="F35" s="13"/>
-    </row>
-    <row r="36" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
-        <v>28</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="7"/>
@@ -1081,7 +1038,7 @@
       <c r="K36" s="7"/>
     </row>
     <row r="37" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
+      <c r="A37" s="16"/>
       <c r="E37" s="12"/>
       <c r="F37" s="13"/>
       <c r="G37" s="8"/>
@@ -1089,8 +1046,8 @@
       <c r="I37" s="8"/>
     </row>
     <row r="38" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
-        <v>29</v>
+      <c r="A38" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="J38" s="11"/>
       <c r="K38" s="12"/>
@@ -1099,7 +1056,7 @@
       <c r="N38" s="9"/>
     </row>
     <row r="39" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+      <c r="A39" s="16"/>
       <c r="J39" s="13"/>
       <c r="K39" s="8"/>
       <c r="L39" s="13"/>
@@ -1107,52 +1064,52 @@
       <c r="N39" s="13"/>
     </row>
     <row r="40" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="O40" s="7"/>
+    </row>
+    <row r="41" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="16"/>
+      <c r="O41" s="8"/>
+    </row>
+    <row r="42" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="O42" s="7"/>
+    </row>
+    <row r="43" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="16"/>
+      <c r="O43" s="8"/>
+    </row>
+    <row r="44" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="O44" s="7"/>
+    </row>
+    <row r="45" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="16"/>
+      <c r="O45" s="8"/>
+    </row>
+    <row r="46" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
         <v>30</v>
-      </c>
-      <c r="O40" s="7"/>
-    </row>
-    <row r="41" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="O41" s="8"/>
-    </row>
-    <row r="42" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="O42" s="7"/>
-    </row>
-    <row r="43" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="O43" s="8"/>
-    </row>
-    <row r="44" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="O44" s="7"/>
-    </row>
-    <row r="45" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="O45" s="8"/>
-    </row>
-    <row r="46" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
-        <v>33</v>
       </c>
       <c r="P46" s="9"/>
       <c r="Q46" s="7"/>
       <c r="R46" s="11"/>
     </row>
     <row r="47" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
+      <c r="A47" s="16"/>
       <c r="P47" s="13"/>
       <c r="Q47" s="8"/>
       <c r="S47" s="8"/>
     </row>
     <row r="48" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
-        <v>38</v>
+      <c r="A48" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="R48" s="9"/>
       <c r="S48" s="7"/>
@@ -1164,15 +1121,15 @@
       <c r="Y48" s="11"/>
     </row>
     <row r="49" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
+      <c r="A49" s="16"/>
       <c r="Q49" s="8"/>
       <c r="R49" s="13"/>
       <c r="X49" s="11"/>
       <c r="Y49" s="11"/>
     </row>
     <row r="50" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
-        <v>39</v>
+      <c r="A50" s="16" t="s">
+        <v>35</v>
       </c>
       <c r="R50" s="11"/>
       <c r="S50" s="12"/>
@@ -1184,15 +1141,17 @@
       <c r="Y50" s="11"/>
     </row>
     <row r="51" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="T51" s="13"/>
+      <c r="A51" s="16"/>
+      <c r="T51" s="11"/>
       <c r="U51" s="8"/>
+      <c r="V51" s="13"/>
+      <c r="W51" s="8"/>
       <c r="X51" s="11"/>
       <c r="Y51" s="11"/>
     </row>
     <row r="52" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
-        <v>34</v>
+      <c r="A52" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="7"/>
@@ -1220,7 +1179,7 @@
       <c r="Y52" s="11"/>
     </row>
     <row r="53" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
+      <c r="A53" s="16"/>
       <c r="B53" s="5"/>
       <c r="C53" s="8"/>
       <c r="D53" s="13"/>
@@ -1241,10 +1200,12 @@
       <c r="S53" s="8"/>
       <c r="T53" s="13"/>
       <c r="U53" s="8"/>
+      <c r="V53" s="13"/>
+      <c r="W53" s="8"/>
     </row>
     <row r="54" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
-        <v>35</v>
+      <c r="A54" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="7"/>
@@ -1270,7 +1231,7 @@
       <c r="W54" s="7"/>
     </row>
     <row r="55" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
+      <c r="A55" s="16"/>
       <c r="B55" s="5"/>
       <c r="C55" s="8"/>
       <c r="D55" s="13"/>
@@ -1291,10 +1252,12 @@
       <c r="S55" s="8"/>
       <c r="T55" s="13"/>
       <c r="U55" s="8"/>
+      <c r="V55" s="13"/>
+      <c r="W55" s="8"/>
     </row>
     <row r="56" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="24"/>
-      <c r="B56" s="25"/>
+      <c r="A56" s="25"/>
+      <c r="B56" s="15"/>
       <c r="C56" s="12"/>
       <c r="D56" s="11"/>
       <c r="E56" s="12"/>
@@ -1318,8 +1281,8 @@
       <c r="W56" s="12"/>
     </row>
     <row r="57" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="24"/>
-      <c r="B57" s="25"/>
+      <c r="A57" s="25"/>
+      <c r="B57" s="15"/>
       <c r="C57" s="12"/>
       <c r="D57" s="11"/>
       <c r="E57" s="12"/>
@@ -1343,42 +1306,36 @@
       <c r="W57" s="12"/>
     </row>
     <row r="58" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
+      <c r="A58" s="16"/>
     </row>
     <row r="59" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
+      <c r="A59" s="16"/>
     </row>
     <row r="60" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
+      <c r="A60" s="16"/>
     </row>
     <row r="61" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
+      <c r="A61" s="16"/>
     </row>
     <row r="62" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="L1:W1"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="R3:S3"/>
@@ -1395,22 +1352,28 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="L1:W1"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>